<commit_message>
Exe 15 - class
</commit_message>
<xml_diff>
--- a/me/1.Lap-trinh-python/8.lap-trinh-huong-doi-tuong.xlsx
+++ b/me/1.Lap-trinh-python/8.lap-trinh-huong-doi-tuong.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vudinhquang/Documents/quang/python/me/1.Lap-trinh-python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07387429-E5B2-A648-99FF-2E9AAE38B574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{377A71DB-AF2A-4347-B91D-2BB4C66D6280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="1500" windowWidth="31700" windowHeight="18660" activeTab="7" xr2:uid="{75036E14-3E0C-CA4B-BD00-0CC048259C31}"/>
+    <workbookView xWindow="2220" yWindow="1500" windowWidth="31700" windowHeight="18660" activeTab="8" xr2:uid="{75036E14-3E0C-CA4B-BD00-0CC048259C31}"/>
   </bookViews>
   <sheets>
     <sheet name="Class" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Str" sheetId="6" r:id="rId6"/>
     <sheet name="len" sheetId="7" r:id="rId7"/>
     <sheet name="del" sheetId="8" r:id="rId8"/>
+    <sheet name="Exe 15 - class" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="205">
   <si>
     <t>構成</t>
   </si>
@@ -639,6 +640,84 @@
   </si>
   <si>
     <t>python3 08_del.py</t>
+  </si>
+  <si>
+    <t>exe_15_class.py</t>
+  </si>
+  <si>
+    <t>python/exe/exe_15_class.py</t>
+  </si>
+  <si>
+    <t>class Course():</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    def __init__(self, name, time, price):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        self.time = time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        self.price = price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        print("Name: {name} - time: {time} - price: {price}".format(</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            name    = self.name, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">            time    = self.time,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            price   = self.price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        ))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        return  "Name: {name} - time: {time} - price: {price}".format(</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        )</t>
+  </si>
+  <si>
+    <t>listCourses = [</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    {'name': 'PHP', 'time': 12, 'price': 20},</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    {'name': 'Django', 'time': 24, 'price': 40}</t>
+  </si>
+  <si>
+    <t>]</t>
+  </si>
+  <si>
+    <t>print(listCourses)</t>
+  </si>
+  <si>
+    <t>result = []</t>
+  </si>
+  <si>
+    <t>for course in listCourses:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    result.append(Course(course["name"],course["time"],course["price"]))</t>
+  </si>
+  <si>
+    <t>for courseObj in result:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    print(courseObj)</t>
+  </si>
+  <si>
+    <t>python3 exe_15_class.py</t>
+  </si>
+  <si>
+    <t>List chứa các Dictionary</t>
+  </si>
+  <si>
+    <t>List chứa các đối tượng</t>
   </si>
 </sst>
 </file>
@@ -2613,6 +2692,166 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>91439</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>92332</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>128962</xdr:colOff>
+      <xdr:row>126</xdr:row>
+      <xdr:rowOff>19428</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{522F2697-316B-07E8-EBCB-046AF56D4F2C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="914399" y="24069932"/>
+          <a:ext cx="11558963" cy="1552696"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>233680</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>172720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>274320</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>111760</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB124D97-1B67-9034-5DF9-63A5AAE0403F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1056640" y="22931120"/>
+          <a:ext cx="40640" cy="1971040"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>640080</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>162560</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>629920</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>132080</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E624434-D39D-F5AA-063F-C5056E741B0F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1463040" y="21295360"/>
+          <a:ext cx="3281680" cy="3423920"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -9952,8 +10191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{108DEF67-2CA8-B646-863F-F8C79FDB5A7A}">
   <dimension ref="A3:K107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="189" workbookViewId="0">
-      <selection activeCell="G95" sqref="G95"/>
+    <sheetView topLeftCell="A53" zoomScale="189" workbookViewId="0">
+      <selection activeCell="J66" sqref="J66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10490,7 +10729,7 @@
       <c r="A49" s="1"/>
       <c r="B49" s="5"/>
       <c r="C49" s="1"/>
-      <c r="D49" s="23" t="s">
+      <c r="D49" t="s">
         <v>156</v>
       </c>
       <c r="E49" s="1"/>
@@ -10801,106 +11040,56 @@
       <c r="B78" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="C78" s="24"/>
-      <c r="D78" s="24"/>
-      <c r="E78" s="24"/>
-      <c r="F78" s="24"/>
-      <c r="G78" s="24"/>
       <c r="H78" s="16"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B79" s="15"/>
-      <c r="C79" s="24"/>
-      <c r="D79" s="24"/>
-      <c r="E79" s="24"/>
-      <c r="F79" s="24"/>
-      <c r="G79" s="24"/>
       <c r="H79" s="16"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B80" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="C80" s="24"/>
-      <c r="D80" s="24"/>
-      <c r="E80" s="24"/>
-      <c r="F80" s="24"/>
-      <c r="G80" s="24"/>
       <c r="H80" s="16"/>
     </row>
     <row r="81" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B81" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="C81" s="24"/>
-      <c r="D81" s="24"/>
-      <c r="E81" s="24"/>
-      <c r="F81" s="24"/>
-      <c r="G81" s="24"/>
       <c r="H81" s="16"/>
     </row>
     <row r="82" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B82" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="C82" s="24"/>
-      <c r="D82" s="24"/>
-      <c r="E82" s="24"/>
-      <c r="F82" s="24"/>
-      <c r="G82" s="24"/>
       <c r="H82" s="16"/>
     </row>
     <row r="83" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B83" s="15"/>
-      <c r="C83" s="24"/>
-      <c r="D83" s="24"/>
-      <c r="E83" s="24"/>
-      <c r="F83" s="24"/>
-      <c r="G83" s="24"/>
       <c r="H83" s="16"/>
     </row>
     <row r="84" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B84" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="C84" s="24"/>
-      <c r="D84" s="24"/>
-      <c r="E84" s="24"/>
-      <c r="F84" s="24"/>
-      <c r="G84" s="24"/>
       <c r="H84" s="16"/>
     </row>
     <row r="85" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B85" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="C85" s="24"/>
-      <c r="D85" s="24"/>
-      <c r="E85" s="24"/>
-      <c r="F85" s="24"/>
-      <c r="G85" s="24"/>
       <c r="H85" s="16"/>
     </row>
     <row r="86" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B86" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="C86" s="24"/>
-      <c r="D86" s="24"/>
-      <c r="E86" s="24"/>
-      <c r="F86" s="24"/>
-      <c r="G86" s="24"/>
       <c r="H86" s="16"/>
     </row>
     <row r="87" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B87" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="C87" s="24"/>
-      <c r="D87" s="24"/>
-      <c r="E87" s="24"/>
-      <c r="F87" s="24"/>
-      <c r="G87" s="24"/>
       <c r="H87" s="16"/>
       <c r="I87" t="s">
         <v>36</v>
@@ -10913,42 +11102,22 @@
       <c r="B88" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="C88" s="24"/>
-      <c r="D88" s="24"/>
-      <c r="E88" s="24"/>
-      <c r="F88" s="24"/>
-      <c r="G88" s="24"/>
       <c r="H88" s="16"/>
     </row>
     <row r="89" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B89" s="15"/>
-      <c r="C89" s="24"/>
-      <c r="D89" s="24"/>
-      <c r="E89" s="24"/>
-      <c r="F89" s="24"/>
-      <c r="G89" s="24"/>
       <c r="H89" s="16"/>
     </row>
     <row r="90" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B90" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="C90" s="24"/>
-      <c r="D90" s="24"/>
-      <c r="E90" s="24"/>
-      <c r="F90" s="24"/>
-      <c r="G90" s="24"/>
       <c r="H90" s="16"/>
     </row>
     <row r="91" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B91" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="C91" s="24"/>
-      <c r="D91" s="24"/>
-      <c r="E91" s="24"/>
-      <c r="F91" s="24"/>
-      <c r="G91" s="24"/>
       <c r="H91" s="16"/>
       <c r="I91" t="s">
         <v>36</v>
@@ -10961,11 +11130,6 @@
       <c r="B92" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="C92" s="24"/>
-      <c r="D92" s="24"/>
-      <c r="E92" s="24"/>
-      <c r="F92" s="24"/>
-      <c r="G92" s="24"/>
       <c r="H92" s="16"/>
       <c r="I92" t="s">
         <v>36</v>
@@ -10978,44 +11142,24 @@
       <c r="B93" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="C93" s="24"/>
-      <c r="D93" s="24"/>
-      <c r="E93" s="24"/>
-      <c r="F93" s="24"/>
-      <c r="G93" s="24"/>
       <c r="H93" s="16"/>
     </row>
     <row r="94" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B94" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="C94" s="24"/>
-      <c r="D94" s="24"/>
-      <c r="E94" s="24"/>
-      <c r="F94" s="24"/>
-      <c r="G94" s="24"/>
       <c r="H94" s="16"/>
     </row>
     <row r="95" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B95" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="C95" s="24"/>
-      <c r="D95" s="24"/>
-      <c r="E95" s="24"/>
-      <c r="F95" s="24"/>
-      <c r="G95" s="24"/>
       <c r="H95" s="16"/>
     </row>
     <row r="96" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B96" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="C96" s="24"/>
-      <c r="D96" s="24"/>
-      <c r="E96" s="24"/>
-      <c r="F96" s="24"/>
-      <c r="G96" s="24"/>
       <c r="H96" s="16"/>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.2">
@@ -11026,12 +11170,6 @@
       <c r="F97" s="18"/>
       <c r="G97" s="18"/>
       <c r="H97" s="19"/>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B98" s="24"/>
-      <c r="C98" s="24"/>
-      <c r="D98" s="24"/>
-      <c r="E98" s="24"/>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100" s="21" t="s">
@@ -11050,82 +11188,29 @@
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101" s="15"/>
-      <c r="B101" s="24" t="s">
+      <c r="B101" t="s">
         <v>178</v>
       </c>
-      <c r="C101" s="24"/>
-      <c r="D101" s="24"/>
-      <c r="E101" s="24"/>
-      <c r="F101" s="24"/>
-      <c r="G101" s="24"/>
-      <c r="H101" s="24"/>
-      <c r="I101" s="24"/>
-      <c r="J101" s="24"/>
       <c r="K101" s="16"/>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" s="15"/>
-      <c r="B102" s="24"/>
-      <c r="C102" s="24"/>
-      <c r="D102" s="24"/>
-      <c r="E102" s="24"/>
-      <c r="F102" s="24"/>
-      <c r="G102" s="24"/>
-      <c r="H102" s="24"/>
-      <c r="I102" s="24"/>
-      <c r="J102" s="24"/>
       <c r="K102" s="16"/>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" s="15"/>
-      <c r="B103" s="24"/>
-      <c r="C103" s="24"/>
-      <c r="D103" s="24"/>
-      <c r="E103" s="24"/>
-      <c r="F103" s="24"/>
-      <c r="G103" s="24"/>
-      <c r="H103" s="24"/>
-      <c r="I103" s="24"/>
-      <c r="J103" s="24"/>
       <c r="K103" s="16"/>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" s="15"/>
-      <c r="B104" s="24"/>
-      <c r="C104" s="24"/>
-      <c r="D104" s="24"/>
-      <c r="E104" s="24"/>
-      <c r="F104" s="24"/>
-      <c r="G104" s="24"/>
-      <c r="H104" s="24"/>
-      <c r="I104" s="24"/>
-      <c r="J104" s="24"/>
       <c r="K104" s="16"/>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105" s="15"/>
-      <c r="B105" s="24"/>
-      <c r="C105" s="24"/>
-      <c r="D105" s="24"/>
-      <c r="E105" s="24"/>
-      <c r="F105" s="24"/>
-      <c r="G105" s="24"/>
-      <c r="H105" s="24"/>
-      <c r="I105" s="24"/>
-      <c r="J105" s="24"/>
       <c r="K105" s="16"/>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" s="15"/>
-      <c r="B106" s="24"/>
-      <c r="C106" s="24"/>
-      <c r="D106" s="24"/>
-      <c r="E106" s="24"/>
-      <c r="F106" s="24"/>
-      <c r="G106" s="24"/>
-      <c r="H106" s="24"/>
-      <c r="I106" s="24"/>
-      <c r="J106" s="24"/>
       <c r="K106" s="16"/>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.2">
@@ -11145,4 +11230,1424 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{238A2DCA-FC2B-A242-881A-943E6FB50F4B}">
+  <dimension ref="A3:P127"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A107" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F132" sqref="F132"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="1"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="1"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="1"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="1"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="1"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="1"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="1"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="1"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="1"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="1"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="1"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="1"/>
+      <c r="D34" t="s">
+        <v>31</v>
+      </c>
+      <c r="E34" s="8"/>
+      <c r="F34" s="6"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="1"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="1"/>
+      <c r="D35" t="s">
+        <v>32</v>
+      </c>
+      <c r="E35" s="8"/>
+      <c r="F35" s="6"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="1"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="1"/>
+      <c r="D36" t="s">
+        <v>33</v>
+      </c>
+      <c r="E36" s="8"/>
+      <c r="F36" s="6"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="1"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E37" s="1"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="1"/>
+      <c r="B38" s="5"/>
+      <c r="C38" t="s">
+        <v>35</v>
+      </c>
+      <c r="E38" s="1"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="1"/>
+      <c r="B39" s="5"/>
+      <c r="D39" t="s">
+        <v>38</v>
+      </c>
+      <c r="E39" s="1"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="1"/>
+      <c r="B40" s="5"/>
+      <c r="D40" t="s">
+        <v>39</v>
+      </c>
+      <c r="E40" s="1"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="1"/>
+      <c r="B41" s="5"/>
+      <c r="D41" t="s">
+        <v>40</v>
+      </c>
+      <c r="E41" s="1"/>
+      <c r="F41" s="6"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="1"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D42" s="8"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="1"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="1"/>
+      <c r="D43" t="s">
+        <v>64</v>
+      </c>
+      <c r="E43" s="1"/>
+      <c r="F43" s="6"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="1"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="1"/>
+      <c r="D44" t="s">
+        <v>79</v>
+      </c>
+      <c r="E44" s="1"/>
+      <c r="F44" s="6"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="1"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="1"/>
+      <c r="D45" t="s">
+        <v>99</v>
+      </c>
+      <c r="E45" s="1"/>
+      <c r="F45" s="6"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="1"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="1"/>
+      <c r="D46" t="s">
+        <v>116</v>
+      </c>
+      <c r="E46" s="1"/>
+      <c r="F46" s="6"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="1"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="1"/>
+      <c r="D47" t="s">
+        <v>125</v>
+      </c>
+      <c r="E47" s="1"/>
+      <c r="F47" s="6"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="1"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="1"/>
+      <c r="D48" t="s">
+        <v>145</v>
+      </c>
+      <c r="E48" s="1"/>
+      <c r="F48" s="6"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="1"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="1"/>
+      <c r="D49" t="s">
+        <v>156</v>
+      </c>
+      <c r="E49" s="1"/>
+      <c r="F49" s="6"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="1"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="E50" s="1"/>
+      <c r="F50" s="6"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="1"/>
+      <c r="B51" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="1"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="1"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="1"/>
+      <c r="D53" t="s">
+        <v>43</v>
+      </c>
+      <c r="E53" s="1"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="1"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="1"/>
+      <c r="D54" t="s">
+        <v>44</v>
+      </c>
+      <c r="E54" s="1"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="1"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="1"/>
+      <c r="D55" t="s">
+        <v>45</v>
+      </c>
+      <c r="E55" s="1"/>
+      <c r="F55" s="6"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" s="1"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="1"/>
+      <c r="D56" t="s">
+        <v>46</v>
+      </c>
+      <c r="E56" s="1"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="1"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="1"/>
+      <c r="D57" t="s">
+        <v>47</v>
+      </c>
+      <c r="E57" s="1"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="1"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E58" s="1"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="1"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="1"/>
+      <c r="B60" s="5"/>
+      <c r="C60" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="1"/>
+      <c r="B61" s="5"/>
+      <c r="C61" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" s="1"/>
+      <c r="B62" s="5"/>
+      <c r="C62" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" s="1"/>
+      <c r="B63" s="5"/>
+      <c r="C63" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" s="1"/>
+      <c r="B64" s="5"/>
+      <c r="C64" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" s="1"/>
+      <c r="B65" s="5"/>
+      <c r="C65" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="1"/>
+      <c r="B66" s="5"/>
+      <c r="C66" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" s="1"/>
+      <c r="B67" s="5"/>
+      <c r="C67" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" s="1"/>
+      <c r="B68" s="5"/>
+      <c r="C68" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="6"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" s="1"/>
+      <c r="B69" s="5"/>
+      <c r="C69" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" s="1"/>
+      <c r="B70" s="5"/>
+      <c r="C70" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="6"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" s="1"/>
+      <c r="B71" s="5"/>
+      <c r="C71" t="s">
+        <v>61</v>
+      </c>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="6"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" s="1"/>
+      <c r="B72" s="5"/>
+      <c r="C72" t="s">
+        <v>62</v>
+      </c>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="6"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" s="1"/>
+      <c r="B73" s="5"/>
+      <c r="C73" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" s="1"/>
+      <c r="B74" s="9"/>
+      <c r="C74" s="10"/>
+      <c r="D74" s="10"/>
+      <c r="E74" s="10"/>
+      <c r="F74" s="11"/>
+      <c r="G74" s="1"/>
+      <c r="H74" s="1"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" s="20" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B78" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="C78" s="13"/>
+      <c r="D78" s="13"/>
+      <c r="E78" s="13"/>
+      <c r="F78" s="13"/>
+      <c r="G78" s="14"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B79" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="C79" s="24"/>
+      <c r="D79" s="24"/>
+      <c r="E79" s="24"/>
+      <c r="F79" s="24"/>
+      <c r="G79" s="16"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B80" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="C80" s="24"/>
+      <c r="D80" s="24"/>
+      <c r="E80" s="24"/>
+      <c r="F80" s="24"/>
+      <c r="G80" s="16"/>
+    </row>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B81" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C81" s="24"/>
+      <c r="D81" s="24"/>
+      <c r="E81" s="24"/>
+      <c r="F81" s="24"/>
+      <c r="G81" s="16"/>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B82" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="C82" s="24"/>
+      <c r="D82" s="24"/>
+      <c r="E82" s="24"/>
+      <c r="F82" s="24"/>
+      <c r="G82" s="16"/>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B83" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="C83" s="24"/>
+      <c r="D83" s="24"/>
+      <c r="E83" s="24"/>
+      <c r="F83" s="24"/>
+      <c r="G83" s="16"/>
+    </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B84" s="15"/>
+      <c r="C84" s="24"/>
+      <c r="D84" s="24"/>
+      <c r="E84" s="24"/>
+      <c r="F84" s="24"/>
+      <c r="G84" s="16"/>
+    </row>
+    <row r="85" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B85" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="C85" s="24"/>
+      <c r="D85" s="24"/>
+      <c r="E85" s="24"/>
+      <c r="F85" s="24"/>
+      <c r="G85" s="16"/>
+    </row>
+    <row r="86" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B86" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="C86" s="24"/>
+      <c r="D86" s="24"/>
+      <c r="E86" s="24"/>
+      <c r="F86" s="24"/>
+      <c r="G86" s="16"/>
+    </row>
+    <row r="87" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B87" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="C87" s="24"/>
+      <c r="D87" s="24"/>
+      <c r="E87" s="24"/>
+      <c r="F87" s="24"/>
+      <c r="G87" s="16"/>
+    </row>
+    <row r="88" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B88" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="C88" s="24"/>
+      <c r="D88" s="24"/>
+      <c r="E88" s="24"/>
+      <c r="F88" s="24"/>
+      <c r="G88" s="16"/>
+    </row>
+    <row r="89" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B89" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="C89" s="24"/>
+      <c r="D89" s="24"/>
+      <c r="E89" s="24"/>
+      <c r="F89" s="24"/>
+      <c r="G89" s="16"/>
+    </row>
+    <row r="90" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B90" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="C90" s="24"/>
+      <c r="D90" s="24"/>
+      <c r="E90" s="24"/>
+      <c r="F90" s="24"/>
+      <c r="G90" s="16"/>
+    </row>
+    <row r="91" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B91" s="15"/>
+      <c r="C91" s="24"/>
+      <c r="D91" s="24"/>
+      <c r="E91" s="24"/>
+      <c r="F91" s="24"/>
+      <c r="G91" s="16"/>
+    </row>
+    <row r="92" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B92" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="C92" s="24"/>
+      <c r="D92" s="24"/>
+      <c r="E92" s="24"/>
+      <c r="F92" s="24"/>
+      <c r="G92" s="16"/>
+    </row>
+    <row r="93" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B93" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="C93" s="24"/>
+      <c r="D93" s="24"/>
+      <c r="E93" s="24"/>
+      <c r="F93" s="24"/>
+      <c r="G93" s="16"/>
+    </row>
+    <row r="94" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B94" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="C94" s="24"/>
+      <c r="D94" s="24"/>
+      <c r="E94" s="24"/>
+      <c r="F94" s="24"/>
+      <c r="G94" s="16"/>
+    </row>
+    <row r="95" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B95" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="C95" s="24"/>
+      <c r="D95" s="24"/>
+      <c r="E95" s="24"/>
+      <c r="F95" s="24"/>
+      <c r="G95" s="16"/>
+    </row>
+    <row r="96" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B96" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="C96" s="24"/>
+      <c r="D96" s="24"/>
+      <c r="E96" s="24"/>
+      <c r="F96" s="24"/>
+      <c r="G96" s="16"/>
+    </row>
+    <row r="97" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B97" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="C97" s="24"/>
+      <c r="D97" s="24"/>
+      <c r="E97" s="24"/>
+      <c r="F97" s="24"/>
+      <c r="G97" s="16"/>
+    </row>
+    <row r="98" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B98" s="15"/>
+      <c r="C98" s="24"/>
+      <c r="D98" s="24"/>
+      <c r="E98" s="24"/>
+      <c r="F98" s="24"/>
+      <c r="G98" s="16"/>
+    </row>
+    <row r="99" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B99" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="C99" s="24"/>
+      <c r="D99" s="24"/>
+      <c r="E99" s="24"/>
+      <c r="F99" s="24"/>
+      <c r="G99" s="16"/>
+      <c r="H99" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I99" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="100" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B100" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="C100" s="24"/>
+      <c r="D100" s="24"/>
+      <c r="E100" s="24"/>
+      <c r="F100" s="24"/>
+      <c r="G100" s="16"/>
+    </row>
+    <row r="101" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B101" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="C101" s="24"/>
+      <c r="D101" s="24"/>
+      <c r="E101" s="24"/>
+      <c r="F101" s="24"/>
+      <c r="G101" s="16"/>
+    </row>
+    <row r="102" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B102" s="15"/>
+      <c r="C102" s="24"/>
+      <c r="D102" s="24"/>
+      <c r="E102" s="24"/>
+      <c r="F102" s="24"/>
+      <c r="G102" s="16"/>
+    </row>
+    <row r="103" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B103" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="C103" s="24"/>
+      <c r="D103" s="24"/>
+      <c r="E103" s="24"/>
+      <c r="F103" s="24"/>
+      <c r="G103" s="16"/>
+    </row>
+    <row r="104" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B104" s="15"/>
+      <c r="C104" s="24"/>
+      <c r="D104" s="24"/>
+      <c r="E104" s="24"/>
+      <c r="F104" s="24"/>
+      <c r="G104" s="16"/>
+    </row>
+    <row r="105" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B105" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="C105" s="24"/>
+      <c r="D105" s="24"/>
+      <c r="E105" s="24"/>
+      <c r="F105" s="24"/>
+      <c r="G105" s="16"/>
+    </row>
+    <row r="106" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B106" s="15"/>
+      <c r="C106" s="24"/>
+      <c r="D106" s="24"/>
+      <c r="E106" s="24"/>
+      <c r="F106" s="24"/>
+      <c r="G106" s="16"/>
+    </row>
+    <row r="107" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B107" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="C107" s="24"/>
+      <c r="D107" s="24"/>
+      <c r="E107" s="24"/>
+      <c r="F107" s="24"/>
+      <c r="G107" s="16"/>
+      <c r="H107" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I107" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="108" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B108" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="C108" s="24"/>
+      <c r="D108" s="24"/>
+      <c r="E108" s="24"/>
+      <c r="F108" s="24"/>
+      <c r="G108" s="16"/>
+    </row>
+    <row r="109" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B109" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="C109" s="24"/>
+      <c r="D109" s="24"/>
+      <c r="E109" s="24"/>
+      <c r="F109" s="24"/>
+      <c r="G109" s="16"/>
+    </row>
+    <row r="110" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B110" s="15"/>
+      <c r="C110" s="24"/>
+      <c r="D110" s="24"/>
+      <c r="E110" s="24"/>
+      <c r="F110" s="24"/>
+      <c r="G110" s="16"/>
+    </row>
+    <row r="111" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B111" s="15"/>
+      <c r="C111" s="24"/>
+      <c r="D111" s="24"/>
+      <c r="E111" s="24"/>
+      <c r="F111" s="24"/>
+      <c r="G111" s="16"/>
+    </row>
+    <row r="112" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B112" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="C112" s="24"/>
+      <c r="D112" s="24"/>
+      <c r="E112" s="24"/>
+      <c r="F112" s="24"/>
+      <c r="G112" s="16"/>
+    </row>
+    <row r="113" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B113" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="C113" s="24"/>
+      <c r="D113" s="24"/>
+      <c r="E113" s="24"/>
+      <c r="F113" s="24"/>
+      <c r="G113" s="16"/>
+    </row>
+    <row r="114" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B114" s="17"/>
+      <c r="C114" s="18"/>
+      <c r="D114" s="18"/>
+      <c r="E114" s="18"/>
+      <c r="F114" s="18"/>
+      <c r="G114" s="19"/>
+    </row>
+    <row r="117" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A117" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="B117" s="13"/>
+      <c r="C117" s="13"/>
+      <c r="D117" s="13"/>
+      <c r="E117" s="13"/>
+      <c r="F117" s="13"/>
+      <c r="G117" s="13"/>
+      <c r="H117" s="13"/>
+      <c r="I117" s="13"/>
+      <c r="J117" s="13"/>
+      <c r="K117" s="13"/>
+      <c r="L117" s="13"/>
+      <c r="M117" s="13"/>
+      <c r="N117" s="13"/>
+      <c r="O117" s="13"/>
+      <c r="P117" s="14"/>
+    </row>
+    <row r="118" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A118" s="15"/>
+      <c r="B118" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="C118" s="24"/>
+      <c r="D118" s="24"/>
+      <c r="E118" s="24"/>
+      <c r="F118" s="24"/>
+      <c r="G118" s="24"/>
+      <c r="H118" s="24"/>
+      <c r="I118" s="24"/>
+      <c r="J118" s="24"/>
+      <c r="K118" s="24"/>
+      <c r="L118" s="24"/>
+      <c r="M118" s="24"/>
+      <c r="N118" s="24"/>
+      <c r="O118" s="24"/>
+      <c r="P118" s="16"/>
+    </row>
+    <row r="119" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A119" s="15"/>
+      <c r="B119" s="24"/>
+      <c r="C119" s="24"/>
+      <c r="D119" s="24"/>
+      <c r="E119" s="24"/>
+      <c r="F119" s="24"/>
+      <c r="G119" s="24"/>
+      <c r="H119" s="24"/>
+      <c r="I119" s="24"/>
+      <c r="J119" s="24"/>
+      <c r="K119" s="24"/>
+      <c r="L119" s="24"/>
+      <c r="M119" s="24"/>
+      <c r="N119" s="24"/>
+      <c r="O119" s="24"/>
+      <c r="P119" s="16"/>
+    </row>
+    <row r="120" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A120" s="15"/>
+      <c r="B120" s="24"/>
+      <c r="C120" s="24"/>
+      <c r="D120" s="24"/>
+      <c r="E120" s="24"/>
+      <c r="F120" s="24"/>
+      <c r="G120" s="24"/>
+      <c r="H120" s="24"/>
+      <c r="I120" s="24"/>
+      <c r="J120" s="24"/>
+      <c r="K120" s="24"/>
+      <c r="L120" s="24"/>
+      <c r="M120" s="24"/>
+      <c r="N120" s="24"/>
+      <c r="O120" s="24"/>
+      <c r="P120" s="16"/>
+    </row>
+    <row r="121" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A121" s="15"/>
+      <c r="B121" s="24"/>
+      <c r="C121" s="24"/>
+      <c r="D121" s="24"/>
+      <c r="E121" s="24"/>
+      <c r="F121" s="24"/>
+      <c r="G121" s="24"/>
+      <c r="H121" s="24"/>
+      <c r="I121" s="24"/>
+      <c r="J121" s="24"/>
+      <c r="K121" s="24"/>
+      <c r="L121" s="24"/>
+      <c r="M121" s="24"/>
+      <c r="N121" s="24"/>
+      <c r="O121" s="24"/>
+      <c r="P121" s="16"/>
+    </row>
+    <row r="122" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A122" s="15"/>
+      <c r="B122" s="24"/>
+      <c r="C122" s="24"/>
+      <c r="D122" s="24"/>
+      <c r="E122" s="24"/>
+      <c r="F122" s="24"/>
+      <c r="G122" s="24"/>
+      <c r="H122" s="24"/>
+      <c r="I122" s="24"/>
+      <c r="J122" s="24"/>
+      <c r="K122" s="24"/>
+      <c r="L122" s="24"/>
+      <c r="M122" s="24"/>
+      <c r="N122" s="24"/>
+      <c r="O122" s="24"/>
+      <c r="P122" s="16"/>
+    </row>
+    <row r="123" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A123" s="15"/>
+      <c r="B123" s="24"/>
+      <c r="C123" s="24"/>
+      <c r="D123" s="24"/>
+      <c r="E123" s="24"/>
+      <c r="F123" s="24"/>
+      <c r="G123" s="24"/>
+      <c r="H123" s="24"/>
+      <c r="I123" s="24"/>
+      <c r="J123" s="24"/>
+      <c r="K123" s="24"/>
+      <c r="L123" s="24"/>
+      <c r="M123" s="24"/>
+      <c r="N123" s="24"/>
+      <c r="O123" s="24"/>
+      <c r="P123" s="16"/>
+    </row>
+    <row r="124" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A124" s="15"/>
+      <c r="B124" s="24"/>
+      <c r="C124" s="24"/>
+      <c r="D124" s="24"/>
+      <c r="E124" s="24"/>
+      <c r="F124" s="24"/>
+      <c r="G124" s="24"/>
+      <c r="H124" s="24"/>
+      <c r="I124" s="24"/>
+      <c r="J124" s="24"/>
+      <c r="K124" s="24"/>
+      <c r="L124" s="24"/>
+      <c r="M124" s="24"/>
+      <c r="N124" s="24"/>
+      <c r="O124" s="24"/>
+      <c r="P124" s="16"/>
+    </row>
+    <row r="125" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A125" s="15"/>
+      <c r="B125" s="24"/>
+      <c r="C125" s="24"/>
+      <c r="D125" s="24"/>
+      <c r="E125" s="24"/>
+      <c r="F125" s="24"/>
+      <c r="G125" s="24"/>
+      <c r="H125" s="24"/>
+      <c r="I125" s="24"/>
+      <c r="J125" s="24"/>
+      <c r="K125" s="24"/>
+      <c r="L125" s="24"/>
+      <c r="M125" s="24"/>
+      <c r="N125" s="24"/>
+      <c r="O125" s="24"/>
+      <c r="P125" s="16"/>
+    </row>
+    <row r="126" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A126" s="15"/>
+      <c r="B126" s="24"/>
+      <c r="C126" s="24"/>
+      <c r="D126" s="24"/>
+      <c r="E126" s="24"/>
+      <c r="F126" s="24"/>
+      <c r="G126" s="24"/>
+      <c r="H126" s="24"/>
+      <c r="I126" s="24"/>
+      <c r="J126" s="24"/>
+      <c r="K126" s="24"/>
+      <c r="L126" s="24"/>
+      <c r="M126" s="24"/>
+      <c r="N126" s="24"/>
+      <c r="O126" s="24"/>
+      <c r="P126" s="16"/>
+    </row>
+    <row r="127" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A127" s="17"/>
+      <c r="B127" s="18"/>
+      <c r="C127" s="18"/>
+      <c r="D127" s="18"/>
+      <c r="E127" s="18"/>
+      <c r="F127" s="18"/>
+      <c r="G127" s="18"/>
+      <c r="H127" s="18"/>
+      <c r="I127" s="18"/>
+      <c r="J127" s="18"/>
+      <c r="K127" s="18"/>
+      <c r="L127" s="18"/>
+      <c r="M127" s="18"/>
+      <c r="N127" s="18"/>
+      <c r="O127" s="18"/>
+      <c r="P127" s="19"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>